<commit_message>
Code for pair trade to deploy on production and added to cron
</commit_message>
<xml_diff>
--- a/data/data_calendarSpreads/ACC.xlsx
+++ b/data/data_calendarSpreads/ACC.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C212"/>
+  <dimension ref="A1:C213"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
       <selection activeCell="A210" sqref="A210:XFD210"/>
@@ -2805,6 +2805,17 @@
         <v>1655</v>
       </c>
     </row>
+    <row r="213">
+      <c r="A213" s="7" t="n">
+        <v>43584.94148581462</v>
+      </c>
+      <c r="B213" t="n">
+        <v>1651.45</v>
+      </c>
+      <c r="C213" t="n">
+        <v>1651.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed downlaod data when lastrecord date is greater than the expiry date
</commit_message>
<xml_diff>
--- a/data/data_calendarSpreads/ACC.xlsx
+++ b/data/data_calendarSpreads/ACC.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C213"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
       <selection activeCell="A210" sqref="A210:XFD210"/>
@@ -2816,6 +2816,17 @@
         <v>1651.2</v>
       </c>
     </row>
+    <row r="214">
+      <c r="A214" s="7" t="n">
+        <v>43585.4894269967</v>
+      </c>
+      <c r="B214" t="n">
+        <v>1642.05</v>
+      </c>
+      <c r="C214" t="n">
+        <v>1648.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>